<commit_message>
update: bereinigtes Abschlussquote-Excel & aktualisiertes Profil-Notebook
</commit_message>
<xml_diff>
--- a/data/bfs_data_abschlussquote.xlsx
+++ b/data/bfs_data_abschlussquote.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\iCloudDrive\Dokumente\02_CLI\Studium\ZHAW\Masterarbeit\vocdata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B125D4-7F77-4467-89D2-B007B2700BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAE5DFC6-DDBF-41C4-9B1E-E0C528C28DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61980" yWindow="1500" windowWidth="21600" windowHeight="12645" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31320" yWindow="1665" windowWidth="25185" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T1_SekII_1st_25_Merkm_Data" sheetId="1" r:id="rId1"/>
     <sheet name="T1_SekII_1st_25_Merkm_Dict" sheetId="2" r:id="rId2"/>
     <sheet name="T2_SekII_1st_25_Kant_Data" sheetId="3" r:id="rId3"/>
-    <sheet name="T2_SekII_1st_25_Kant_Dict." sheetId="4" r:id="rId4"/>
-    <sheet name="T3_Matura_Merkm_data" sheetId="5" r:id="rId5"/>
-    <sheet name="T3_Matura_Merk_dict" sheetId="6" r:id="rId6"/>
-    <sheet name="T4_Matura_Kant_data" sheetId="7" r:id="rId7"/>
-    <sheet name="T4_Matura_Kant_dict" sheetId="8" r:id="rId8"/>
+    <sheet name="T2_SekII_1st_25_Kant_Dict" sheetId="4" r:id="rId4"/>
+    <sheet name="T3_Matura_Merkm_Data" sheetId="5" r:id="rId5"/>
+    <sheet name="T3_Matura_Merk_Dict" sheetId="6" r:id="rId6"/>
+    <sheet name="T4_Matura_Kant_Data" sheetId="7" r:id="rId7"/>
+    <sheet name="T4_Matura_Kant_Dict" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1203,7 +1203,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2247,7 +2247,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C15" sqref="C15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2388,7 +2388,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2932,7 +2932,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3055,7 +3055,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4134,7 +4134,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>